<commit_message>
Teachers and auditories data is fixed in excel files
</commit_message>
<xml_diff>
--- a/data/Departments.xlsx
+++ b/data/Departments.xlsx
@@ -798,7 +798,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -808,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C72" sqref="A68:C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>

</xml_diff>